<commit_message>
a few changes to main func to parse chat outputs into table
</commit_message>
<xml_diff>
--- a/results/output.xlsx
+++ b/results/output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinzhao/DS_Projects/semiauto-epi-data-extraction-pipeline/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05E3211-F6D8-2844-8F20-D0DC5BAC677F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F998F4-E924-1049-A572-5F24DF0A5D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1084,8 +1084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
applied date normalization func
</commit_message>
<xml_diff>
--- a/results/output.xlsx
+++ b/results/output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinzhao/DS_Projects/semiauto-epi-data-extraction-pipeline/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC5F5F9-2485-AC4A-9BC1-222080FFED63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6F6214-D93E-F645-B0E0-281595C1B5F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -244,10 +244,10 @@
     <t>Retrospective cohort study</t>
   </si>
   <si>
-    <t>2011</t>
-  </si>
-  <si>
-    <t>2019</t>
+    <t>December 31, 2011</t>
+  </si>
+  <si>
+    <t>December 31, 2019</t>
   </si>
   <si>
     <t>Patients with genetically confirmed CMS</t>
@@ -259,10 +259,10 @@
     <t>Patients referred for neuromuscular disorders</t>
   </si>
   <si>
-    <t>2010</t>
-  </si>
-  <si>
-    <t>1999</t>
+    <t>January 1, 2010</t>
+  </si>
+  <si>
+    <t>January 1, 1999</t>
   </si>
   <si>
     <t>Retrospective</t>
@@ -647,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:Y4"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -673,9 +673,9 @@
     <col min="18" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="36" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="4.1640625" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>